<commit_message>
letshope this is almost done
</commit_message>
<xml_diff>
--- a/questionnaires/RBDstandardized_questionnaireFCSFCSN_FR.xlsx
+++ b/questionnaires/RBDstandardized_questionnaireFCSFCSN_FR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RBD_Resilience_guide_FR\questionnaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE714BF4-BEEF-472A-8720-BF88C85A1190}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD20FA0-F7F4-4D06-B3E0-38F4BD8F54E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{E25D54C6-3086-4347-8310-63AD65021B04}"/>
+    <workbookView xWindow="20370" yWindow="-1545" windowWidth="25440" windowHeight="15390" xr2:uid="{E25D54C6-3086-4347-8310-63AD65021B04}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$N$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$N$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="105">
   <si>
     <t>type</t>
   </si>
@@ -97,9 +97,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>select_one Yesno</t>
-  </si>
-  <si>
     <t>select_one SRf</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
   </si>
   <si>
     <t>FCSDairy</t>
-  </si>
-  <si>
-    <t>HDDSDairy</t>
   </si>
   <si>
     <t>FCSDairySRf</t>
@@ -411,91 +405,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Au cours des 7 derniers jours, combien de jours les membres de votre ménage ont-ils mangé/buvé: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Le lait et les produits laitiers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, tels que : (lait frais / aigre, yaourt, fromage, autres produits laitiers </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>remplacer par des exemples localement pertinents</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>)   sauf margarine / beurre ou de petites quantités de lait pour le thé / café ?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Hier, pendant la journée et la nuit, les membres de votre ménage ont-ils mangé 
- </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Le lait et les produits laitiers,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> tels que : (lait frais / aigre, yaourt, fromage, autres produits laitiers </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>remplacer par des exemples localement pertinents</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>)   sauf margarine / beurre ou de petites quantités de lait pour le thé / café ?</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Au cours des 7 derniers jours, quelle a été la source principale de 
 </t>
     </r>
@@ -1376,22 +1285,52 @@
     </r>
   </si>
   <si>
-    <t>lhcslt</t>
-  </si>
-  <si>
-    <t>Non, je n'ai pas été confronté à une insuffisance de nourriture</t>
-  </si>
-  <si>
-    <t>Non, parce que j’ai déjà vendu ces actifs ou mené cette activité au cours des 12 derniers mois et je ne peux pas continuer à le faire</t>
-  </si>
-  <si>
-    <t>Non applicable</t>
-  </si>
-  <si>
     <t>FCSPrSRf</t>
   </si>
   <si>
     <t>Francais</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Au cours des 7 derniers jours, combien de jours les membres de votre ménage ont-ils mangé/bu: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Le lait et les produits laitiers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, tels que : (lait frais / aigre, yaourt, fromage, autres produits laitiers </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>remplacer par des exemples localement pertinents</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)   sauf margarine / beurre ou de petites quantités de lait pour le thé / café ?</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1505,7 +1444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1560,10 +1499,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1885,10 +1820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7AFB159-24AC-4874-85C9-2F1DE42CCCC7}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="63" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1945,14 +1880,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="8" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="23" t="s">
+      <c r="A2" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>55</v>
+      <c r="C2" s="22" t="s">
+        <v>53</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -1971,10 +1906,10 @@
         <v>15</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
@@ -1996,13 +1931,13 @@
     </row>
     <row r="4" spans="1:14" s="10" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -2013,7 +1948,7 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
@@ -2025,10 +1960,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
@@ -2046,13 +1981,13 @@
     </row>
     <row r="6" spans="1:14" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -2063,7 +1998,7 @@
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="63" customHeight="1" x14ac:dyDescent="0.2">
@@ -2071,10 +2006,10 @@
         <v>15</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="7" t="s">
@@ -2091,14 +2026,14 @@
       <c r="J7" s="17"/>
     </row>
     <row r="8" spans="1:14" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>24</v>
+      <c r="B8" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -2109,68 +2044,69 @@
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
       <c r="J8" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>17</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="11" t="s">
         <v>18</v>
       </c>
+      <c r="J10" s="11" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>110</v>
+        <v>25</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="G11" s="11" t="s">
         <v>18</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="63" customHeight="1" x14ac:dyDescent="0.2">
@@ -2178,22 +2114,22 @@
         <v>15</v>
       </c>
       <c r="B12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>29</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>18</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="63" customHeight="1" x14ac:dyDescent="0.2">
@@ -2201,22 +2137,22 @@
         <v>15</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>18</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="63" customHeight="1" x14ac:dyDescent="0.2">
@@ -2224,84 +2160,84 @@
         <v>15</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>82</v>
+        <v>31</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>79</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>18</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>29</v>
+      <c r="B15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="11" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="16" spans="1:14" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>15</v>
+      <c r="A16" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>17</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
       <c r="G16" s="11" t="s">
         <v>18</v>
       </c>
+      <c r="J16" s="11" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>102</v>
+        <v>15</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="G17" s="11" t="s">
         <v>18</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
@@ -2309,224 +2245,196 @@
         <v>15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>85</v>
+        <v>34</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>54</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>18</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>29</v>
+      <c r="B19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="11" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="20" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>17</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
       <c r="G20" s="11" t="s">
         <v>18</v>
       </c>
+      <c r="J20" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="21" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>104</v>
+      <c r="A21" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+        <v>83</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="G21" s="11" t="s">
         <v>18</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>38</v>
+      <c r="B22" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>29</v>
+        <v>84</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J22" s="11" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="23" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>39</v>
+        <v>19</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>18</v>
       </c>
+      <c r="J23" s="11" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="24" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>40</v>
+        <v>15</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>89</v>
+        <v>86</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J24" s="11" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="25" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>18</v>
       </c>
+      <c r="J25" s="11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="26" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>42</v>
+        <v>15</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J26" s="11" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="27" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J28" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="21"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
+      <c r="J27" s="11" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2536,17 +2444,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0138E845-9786-443D-9180-88293D55D895}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A6" sqref="A6:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2557,181 +2465,137 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" s="4">
         <v>100</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" s="4">
         <v>200</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" s="4">
         <v>300</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B9" s="4">
         <v>400</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B10" s="4">
         <v>500</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11" s="4">
         <v>600</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" s="4">
         <v>700</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" s="4">
         <v>800</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B14" s="4">
         <v>900</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B15" s="4">
         <v>1000</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>106</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>106</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>106</v>
-      </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>106</v>
-      </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2743,7 +2607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FBF12F9-1149-46D7-A16F-F12529849F44}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2754,24 +2618,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>